<commit_message>
Objective Functions for Ownership
Can now vary objective functions
</commit_message>
<xml_diff>
--- a/Input/Optimization Parameters Table Demo.xlsx
+++ b/Input/Optimization Parameters Table Demo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Objective Function</t>
+  </si>
+  <si>
+    <t>Maximize Points</t>
+  </si>
+  <si>
+    <t>Maximize Ownership</t>
+  </si>
+  <si>
+    <t>Minimize Ownership</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
+    <t>Scenario4</t>
+  </si>
+  <si>
+    <t>Scenario5</t>
+  </si>
+  <si>
+    <t>Scenario6</t>
   </si>
 </sst>
 </file>
@@ -129,8 +153,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,11 +200,23 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -461,9 +509,10 @@
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="42">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="42">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -482,13 +531,16 @@
       <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2" s="8">
         <v>5</v>
@@ -502,13 +554,16 @@
       <c r="F2" s="9">
         <v>2</v>
       </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C3" s="8">
         <v>5</v>
@@ -522,12 +577,101 @@
       <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="C4"/>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="C5"/>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="8">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>